<commit_message>
Configuration parameter values sync
</commit_message>
<xml_diff>
--- a/tests/fixtures/comparation_product.xlsx
+++ b/tests/fixtures/comparation_product.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marc1/Documents/Connect/connect-cli/tests/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44A38A7C-11D6-B341-AE4F-7982F5C7E992}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9649BED8-1AEF-2B40-88A6-543DB0C315DE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37440" yWindow="500" windowWidth="35840" windowHeight="20720" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="500" windowWidth="35840" windowHeight="20720" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General Information" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="785" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="823" uniqueCount="332">
   <si>
     <t>Product information</t>
   </si>
@@ -1035,9 +1035,6 @@
     <t>Parameter</t>
   </si>
   <si>
-    <t>Item</t>
-  </si>
-  <si>
     <t>Marketplace</t>
   </si>
   <si>
@@ -1162,6 +1159,15 @@
   </si>
   <si>
     <t>2020-11-27T08:37:16+00:00</t>
+  </si>
+  <si>
+    <t>Item ID</t>
+  </si>
+  <si>
+    <t>Item Name</t>
+  </si>
+  <si>
+    <t>Marketplace Name</t>
   </si>
 </sst>
 </file>
@@ -1229,7 +1235,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1247,6 +1253,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1568,10 +1575,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="31" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
+      <c r="B1" s="13"/>
     </row>
     <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
@@ -1769,16 +1776,22 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:H1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="7" width="25" bestFit="1" customWidth="1"/>
+    <col min="1" max="5" width="25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>53</v>
       </c>
@@ -1792,18 +1805,24 @@
         <v>24</v>
       </c>
       <c r="E1" s="7" t="s">
+        <v>329</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>330</v>
+      </c>
+      <c r="G1" s="7" t="s">
         <v>287</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="H1" s="7" t="s">
+        <v>331</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>288</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>289</v>
       </c>
       <c r="B2" t="s">
         <v>274</v>
@@ -1817,16 +1836,22 @@
       <c r="E2" t="s">
         <v>91</v>
       </c>
-      <c r="F2" t="s">
-        <v>27</v>
+      <c r="F2" s="11" t="s">
+        <v>93</v>
       </c>
       <c r="G2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>290</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>291</v>
       </c>
       <c r="B3" t="s">
         <v>274</v>
@@ -1840,16 +1865,22 @@
       <c r="E3" t="s">
         <v>101</v>
       </c>
-      <c r="F3" t="s">
-        <v>27</v>
+      <c r="F3" s="11" t="s">
+        <v>103</v>
       </c>
       <c r="G3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H3" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B4" t="s">
         <v>274</v>
@@ -1863,16 +1894,22 @@
       <c r="E4" t="s">
         <v>106</v>
       </c>
-      <c r="F4" t="s">
-        <v>27</v>
+      <c r="F4" s="11" t="s">
+        <v>108</v>
       </c>
       <c r="G4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H4" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B5" t="s">
         <v>274</v>
@@ -1886,16 +1923,22 @@
       <c r="E5" t="s">
         <v>111</v>
       </c>
-      <c r="F5" t="s">
-        <v>27</v>
+      <c r="F5" s="11" t="s">
+        <v>113</v>
       </c>
       <c r="G5" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H5" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B6" t="s">
         <v>274</v>
@@ -1909,16 +1952,22 @@
       <c r="E6" t="s">
         <v>116</v>
       </c>
-      <c r="F6" t="s">
-        <v>27</v>
+      <c r="F6" s="11" t="s">
+        <v>118</v>
       </c>
       <c r="G6" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H6" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B7" t="s">
         <v>274</v>
@@ -1932,16 +1981,22 @@
       <c r="E7" t="s">
         <v>121</v>
       </c>
-      <c r="F7" t="s">
-        <v>27</v>
+      <c r="F7" s="11" t="s">
+        <v>123</v>
       </c>
       <c r="G7" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H7" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B8" t="s">
         <v>274</v>
@@ -1955,16 +2010,22 @@
       <c r="E8" t="s">
         <v>126</v>
       </c>
-      <c r="F8" t="s">
-        <v>27</v>
+      <c r="F8" s="11" t="s">
+        <v>128</v>
       </c>
       <c r="G8" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H8" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B9" t="s">
         <v>274</v>
@@ -1978,16 +2039,22 @@
       <c r="E9" t="s">
         <v>131</v>
       </c>
-      <c r="F9" t="s">
-        <v>27</v>
+      <c r="F9" s="11" t="s">
+        <v>133</v>
       </c>
       <c r="G9" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H9" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B10" t="s">
         <v>274</v>
@@ -2001,16 +2068,22 @@
       <c r="E10" t="s">
         <v>136</v>
       </c>
-      <c r="F10" t="s">
-        <v>27</v>
+      <c r="F10" s="11" t="s">
+        <v>138</v>
       </c>
       <c r="G10" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H10" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B11" t="s">
         <v>274</v>
@@ -2024,16 +2097,22 @@
       <c r="E11" t="s">
         <v>141</v>
       </c>
-      <c r="F11" t="s">
-        <v>27</v>
+      <c r="F11" s="11" t="s">
+        <v>143</v>
       </c>
       <c r="G11" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H11" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B12" t="s">
         <v>274</v>
@@ -2047,16 +2126,22 @@
       <c r="E12" t="s">
         <v>146</v>
       </c>
-      <c r="F12" t="s">
-        <v>27</v>
+      <c r="F12" s="11" t="s">
+        <v>148</v>
       </c>
       <c r="G12" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H12" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B13" t="s">
         <v>274</v>
@@ -2070,16 +2155,22 @@
       <c r="E13" t="s">
         <v>151</v>
       </c>
-      <c r="F13" t="s">
-        <v>27</v>
+      <c r="F13" s="11" t="s">
+        <v>153</v>
       </c>
       <c r="G13" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H13" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B14" t="s">
         <v>274</v>
@@ -2093,16 +2184,22 @@
       <c r="E14" t="s">
         <v>156</v>
       </c>
-      <c r="F14" t="s">
-        <v>27</v>
+      <c r="F14" s="11" t="s">
+        <v>158</v>
       </c>
       <c r="G14" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H14" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B15" t="s">
         <v>274</v>
@@ -2116,16 +2213,22 @@
       <c r="E15" t="s">
         <v>161</v>
       </c>
-      <c r="F15" t="s">
-        <v>27</v>
+      <c r="F15" s="11" t="s">
+        <v>163</v>
       </c>
       <c r="G15" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H15" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B16" t="s">
         <v>274</v>
@@ -2139,16 +2242,22 @@
       <c r="E16" t="s">
         <v>166</v>
       </c>
-      <c r="F16" t="s">
-        <v>27</v>
+      <c r="F16" s="11" t="s">
+        <v>168</v>
       </c>
       <c r="G16" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H16" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B17" t="s">
         <v>274</v>
@@ -2162,16 +2271,22 @@
       <c r="E17" t="s">
         <v>171</v>
       </c>
-      <c r="F17" t="s">
-        <v>27</v>
+      <c r="F17" s="11" t="s">
+        <v>173</v>
       </c>
       <c r="G17" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H17" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B18" t="s">
         <v>274</v>
@@ -2185,16 +2300,22 @@
       <c r="E18" t="s">
         <v>176</v>
       </c>
-      <c r="F18" t="s">
-        <v>27</v>
+      <c r="F18" s="11" t="s">
+        <v>178</v>
       </c>
       <c r="G18" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H18" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B19" t="s">
         <v>274</v>
@@ -2208,16 +2329,22 @@
       <c r="E19" t="s">
         <v>181</v>
       </c>
-      <c r="F19" t="s">
-        <v>27</v>
+      <c r="F19" s="11" t="s">
+        <v>183</v>
       </c>
       <c r="G19" t="s">
+        <v>27</v>
+      </c>
+      <c r="H19" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I19" t="s">
         <v>27</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D2 D3 D4 D5 D6 D7 D8 D9 D10 D11 D12 D13 D14 D15 D16 D17 D18 D19" xr:uid="{00000000-0002-0000-0A00-000000000000}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D2:D19" xr:uid="{00000000-0002-0000-0A00-000000000000}">
       <formula1>"-,create,update,delete"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2647,10 +2774,10 @@
         <v>70</v>
       </c>
       <c r="G2" s="8" t="s">
+        <v>311</v>
+      </c>
+      <c r="H2" s="8" t="s">
         <v>312</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -2673,10 +2800,10 @@
         <v>74</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="144" x14ac:dyDescent="0.2">
@@ -2699,10 +2826,10 @@
         <v>77</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="144" x14ac:dyDescent="0.2">
@@ -2725,10 +2852,10 @@
         <v>80</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
   </sheetData>
@@ -3563,7 +3690,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A43BD51-F0A3-C041-B921-6AA80B1D516A}">
   <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3655,10 +3782,10 @@
         <v>199</v>
       </c>
       <c r="M2" s="8" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="N2" s="8" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="96" x14ac:dyDescent="0.2">
@@ -3699,10 +3826,10 @@
         <v>205</v>
       </c>
       <c r="M3" s="8" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="N3" s="8" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="288" x14ac:dyDescent="0.2">
@@ -3743,10 +3870,10 @@
         <v>211</v>
       </c>
       <c r="M4" s="8" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N4" s="8" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="304" x14ac:dyDescent="0.2">
@@ -3787,10 +3914,10 @@
         <v>217</v>
       </c>
       <c r="M5" s="8" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="N5" s="8" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="80" x14ac:dyDescent="0.2">
@@ -3831,10 +3958,10 @@
         <v>199</v>
       </c>
       <c r="M6" s="8" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="N6" s="8" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="320" x14ac:dyDescent="0.2">
@@ -3875,10 +4002,10 @@
         <v>228</v>
       </c>
       <c r="M7" s="8" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="N7" s="8" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="64" x14ac:dyDescent="0.2">
@@ -3919,10 +4046,10 @@
         <v>234</v>
       </c>
       <c r="M8" s="8" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="N8" s="8" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="96" x14ac:dyDescent="0.2">
@@ -3963,10 +4090,10 @@
         <v>240</v>
       </c>
       <c r="M9" s="8" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="N9" s="8" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="112" x14ac:dyDescent="0.2">
@@ -4007,10 +4134,10 @@
         <v>246</v>
       </c>
       <c r="M10" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="N10" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="80" x14ac:dyDescent="0.2">
@@ -4051,10 +4178,10 @@
         <v>199</v>
       </c>
       <c r="M11" s="8" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="N11" s="8" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="256" x14ac:dyDescent="0.2">
@@ -4095,10 +4222,10 @@
         <v>257</v>
       </c>
       <c r="M12" s="8" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="N12" s="8" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="80" x14ac:dyDescent="0.2">
@@ -4139,10 +4266,10 @@
         <v>199</v>
       </c>
       <c r="M13" s="8" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="N13" s="8" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
   </sheetData>
@@ -4263,10 +4390,10 @@
         <v>267</v>
       </c>
       <c r="M2" s="8" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="N2" s="8" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="112" x14ac:dyDescent="0.2">
@@ -4307,10 +4434,10 @@
         <v>272</v>
       </c>
       <c r="M3" s="8" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="N3" s="8" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
   </sheetData>
@@ -4431,10 +4558,10 @@
         <v>277</v>
       </c>
       <c r="M2" s="8" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="N2" s="8" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed capabilities sync for future and dynamic items, fixed tier1 and tier2 templates sync
</commit_message>
<xml_diff>
--- a/tests/fixtures/comparation_product.xlsx
+++ b/tests/fixtures/comparation_product.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marc1/Documents/Connect/connect-cli/tests/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B5B8ADF-3553-0F47-9238-EAA602CACC74}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2189059-0C73-074E-869B-7996F038FC52}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36140" yWindow="500" windowWidth="35840" windowHeight="20720" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="36140" yWindow="500" windowWidth="35840" windowHeight="20720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General Information" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="825" uniqueCount="332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="835" uniqueCount="337">
   <si>
     <t>Product information</t>
   </si>
@@ -1168,6 +1168,21 @@
   </si>
   <si>
     <t>Marketplace ID</t>
+  </si>
+  <si>
+    <t>TL-559-508-354</t>
+  </si>
+  <si>
+    <t>Default Activation Template</t>
+  </si>
+  <si>
+    <t>tier1</t>
+  </si>
+  <si>
+    <t>TL-518-222-757</t>
+  </si>
+  <si>
+    <t>tier2</t>
   </si>
 </sst>
 </file>
@@ -1229,7 +1244,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1246,6 +1261,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1568,10 +1584,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="31" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
+      <c r="B1" s="13"/>
     </row>
     <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
@@ -1779,7 +1795,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
@@ -2713,10 +2729,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3134AC6-DDEE-044F-825B-D4DF0F5E2D02}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2781,64 +2797,52 @@
         <v>311</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
-        <v>71</v>
+        <v>332</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>72</v>
+        <v>333</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>27</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>68</v>
+        <v>334</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>310</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="144" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+      <c r="F3" s="5"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+    </row>
+    <row r="4" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>75</v>
+        <v>335</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>76</v>
+        <v>333</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>27</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>68</v>
+        <v>336</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="F4" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>309</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="144" x14ac:dyDescent="0.2">
+      <c r="F4" s="5"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+    </row>
+    <row r="5" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>27</v>
@@ -2847,27 +2851,79 @@
         <v>68</v>
       </c>
       <c r="E5" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="144" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E6" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F6" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>309</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="144" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G7" s="7" t="s">
         <v>307</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="H7" s="7" t="s">
         <v>306</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E2:E5" xr:uid="{00000000-0002-0000-0400-000002000000}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E2:E7" xr:uid="{00000000-0002-0000-0400-000002000000}">
       <formula1>"fulfillment,inquire"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D2:D5" xr:uid="{00000000-0002-0000-0400-000001000000}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D2:D7" xr:uid="{00000000-0002-0000-0400-000001000000}">
       <formula1>"asset,tier1,tier2"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C5" xr:uid="{00000000-0002-0000-0400-000000000000}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C7" xr:uid="{00000000-0002-0000-0400-000000000000}">
       <formula1>"-,create,update,delete"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
LITE-22868: Include primary locale on product export and cloning
</commit_message>
<xml_diff>
--- a/tests/fixtures/comparation_product.xlsx
+++ b/tests/fixtures/comparation_product.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marc1/Documents/Connect/connect-cli/tests/fixtures/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carlosherrero/projects/connect-cli/tests/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2189059-0C73-074E-869B-7996F038FC52}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E12F042C-4FCA-6B48-9E1E-D06C0AAD913E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36140" yWindow="500" windowWidth="35840" windowHeight="20720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General Information" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="835" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="436">
   <si>
     <t>Product information</t>
   </si>
@@ -1184,12 +1184,309 @@
   <si>
     <t>tier2</t>
   </si>
+  <si>
+    <t>Locales</t>
+  </si>
+  <si>
+    <t>AF (Afrikaans)</t>
+  </si>
+  <si>
+    <t>AR (Arabic)</t>
+  </si>
+  <si>
+    <t>AR-DZ (Algerian Arabic)</t>
+  </si>
+  <si>
+    <t>AST (Asturian)</t>
+  </si>
+  <si>
+    <t>AZ (Azerbaijani)</t>
+  </si>
+  <si>
+    <t>BE (Belarusian)</t>
+  </si>
+  <si>
+    <t>BG (Bulgarian)</t>
+  </si>
+  <si>
+    <t>BN (Bengali)</t>
+  </si>
+  <si>
+    <t>BR (Breton)</t>
+  </si>
+  <si>
+    <t>BS (Bosnian)</t>
+  </si>
+  <si>
+    <t>CA (Catalan)</t>
+  </si>
+  <si>
+    <t>CS (Czech)</t>
+  </si>
+  <si>
+    <t>CY (Welsh)</t>
+  </si>
+  <si>
+    <t>DA (Danish)</t>
+  </si>
+  <si>
+    <t>DE (German)</t>
+  </si>
+  <si>
+    <t>DSB (Lower Sorbian)</t>
+  </si>
+  <si>
+    <t>EL (Greek)</t>
+  </si>
+  <si>
+    <t>EN (English)</t>
+  </si>
+  <si>
+    <t>EN-AU (Australian English)</t>
+  </si>
+  <si>
+    <t>EN-GB (British English)</t>
+  </si>
+  <si>
+    <t>EO (Esperanto)</t>
+  </si>
+  <si>
+    <t>ES (Spanish)</t>
+  </si>
+  <si>
+    <t>ES-AR (Argentinian Spanish)</t>
+  </si>
+  <si>
+    <t>ES-CO (Colombian Spanish)</t>
+  </si>
+  <si>
+    <t>ES-MX (Mexican Spanish)</t>
+  </si>
+  <si>
+    <t>ES-NI (Nicaraguan Spanish)</t>
+  </si>
+  <si>
+    <t>ES-VE (Venezuelan Spanish)</t>
+  </si>
+  <si>
+    <t>ET (Estonian)</t>
+  </si>
+  <si>
+    <t>EU (Basque)</t>
+  </si>
+  <si>
+    <t>FA (Persian)</t>
+  </si>
+  <si>
+    <t>FI (Finnish)</t>
+  </si>
+  <si>
+    <t>FR (French)</t>
+  </si>
+  <si>
+    <t>FY (Frisian)</t>
+  </si>
+  <si>
+    <t>GA (Irish)</t>
+  </si>
+  <si>
+    <t>GD (Scottish Gaelic)</t>
+  </si>
+  <si>
+    <t>GL (Galician)</t>
+  </si>
+  <si>
+    <t>HE (Hebrew)</t>
+  </si>
+  <si>
+    <t>HI (Hindi)</t>
+  </si>
+  <si>
+    <t>HR (Croatian)</t>
+  </si>
+  <si>
+    <t>HSB (Upper Sorbian)</t>
+  </si>
+  <si>
+    <t>HU (Hungarian)</t>
+  </si>
+  <si>
+    <t>HY (Armenian)</t>
+  </si>
+  <si>
+    <t>IA (Interlingua)</t>
+  </si>
+  <si>
+    <t>ID (Indonesian)</t>
+  </si>
+  <si>
+    <t>IG (Igbo)</t>
+  </si>
+  <si>
+    <t>IO (Ido)</t>
+  </si>
+  <si>
+    <t>IS (Icelandic)</t>
+  </si>
+  <si>
+    <t>IT (Italian)</t>
+  </si>
+  <si>
+    <t>JA (Japanese)</t>
+  </si>
+  <si>
+    <t>KA (Georgian)</t>
+  </si>
+  <si>
+    <t>KAB (Kabyle)</t>
+  </si>
+  <si>
+    <t>KK (Kazakh)</t>
+  </si>
+  <si>
+    <t>KM (Khmer)</t>
+  </si>
+  <si>
+    <t>KN (Kannada)</t>
+  </si>
+  <si>
+    <t>KO (Korean)</t>
+  </si>
+  <si>
+    <t>KY (Kyrgyz)</t>
+  </si>
+  <si>
+    <t>LB (Luxembourgish)</t>
+  </si>
+  <si>
+    <t>LT (Lithuanian)</t>
+  </si>
+  <si>
+    <t>LV (Latvian)</t>
+  </si>
+  <si>
+    <t>MK (Macedonian)</t>
+  </si>
+  <si>
+    <t>ML (Malayalam)</t>
+  </si>
+  <si>
+    <t>MN (Mongolian)</t>
+  </si>
+  <si>
+    <t>MR (Marathi)</t>
+  </si>
+  <si>
+    <t>MY (Burmese)</t>
+  </si>
+  <si>
+    <t>NB (Norwegian Bokmal)</t>
+  </si>
+  <si>
+    <t>NE (Nepali)</t>
+  </si>
+  <si>
+    <t>NL (Dutch)</t>
+  </si>
+  <si>
+    <t>NN (Norwegian Nynorsk)</t>
+  </si>
+  <si>
+    <t>NO (Norwegian)</t>
+  </si>
+  <si>
+    <t>OS (Ossetic)</t>
+  </si>
+  <si>
+    <t>PA (Punjabi)</t>
+  </si>
+  <si>
+    <t>PL (Polish)</t>
+  </si>
+  <si>
+    <t>PT (Portuguese)</t>
+  </si>
+  <si>
+    <t>PT-BR (Brazilian Portuguese)</t>
+  </si>
+  <si>
+    <t>RO (Romanian)</t>
+  </si>
+  <si>
+    <t>RU (Russian)</t>
+  </si>
+  <si>
+    <t>SK (Slovak)</t>
+  </si>
+  <si>
+    <t>SL (Slovenian)</t>
+  </si>
+  <si>
+    <t>SQ (Albanian)</t>
+  </si>
+  <si>
+    <t>SR (Serbian)</t>
+  </si>
+  <si>
+    <t>SR-LATN (Serbian Latin)</t>
+  </si>
+  <si>
+    <t>SV (Swedish)</t>
+  </si>
+  <si>
+    <t>SW (Swahili)</t>
+  </si>
+  <si>
+    <t>TA (Tamil)</t>
+  </si>
+  <si>
+    <t>TE (Telugu)</t>
+  </si>
+  <si>
+    <t>TG (Tajik)</t>
+  </si>
+  <si>
+    <t>TH (Thai)</t>
+  </si>
+  <si>
+    <t>TK (Turkmen)</t>
+  </si>
+  <si>
+    <t>TR (Turkish)</t>
+  </si>
+  <si>
+    <t>TT (Tatar)</t>
+  </si>
+  <si>
+    <t>UDM (Udmurt)</t>
+  </si>
+  <si>
+    <t>UK (Ukrainian)</t>
+  </si>
+  <si>
+    <t>UR (Urdu)</t>
+  </si>
+  <si>
+    <t>UZ (Uzbek)</t>
+  </si>
+  <si>
+    <t>VI (Vietnamese)</t>
+  </si>
+  <si>
+    <t>ZH-HANS (Simplified Chinese)</t>
+  </si>
+  <si>
+    <t>ZH-HANT (Traditional Chinese)</t>
+  </si>
+  <si>
+    <t>Primary Translation Locale</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1212,6 +1509,13 @@
       <sz val="14"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1244,7 +1548,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1265,6 +1569,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1571,10 +1877,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:AB98"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1583,107 +1889,582 @@
     <col min="2" max="2" width="180" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="31" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:28" ht="31" x14ac:dyDescent="0.2">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-    </row>
-    <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="B1" s="15"/>
+      <c r="AB1" s="12" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AB2" s="12" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="AB3" s="12" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="AB4" s="12" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="AB5" s="12" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="AB6" s="12" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="AB7" s="12" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" ht="19" x14ac:dyDescent="0.25">
+      <c r="AB8" s="12" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" ht="19" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="AB9" s="12" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" ht="404" x14ac:dyDescent="0.2">
+      <c r="AB10" s="12" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" ht="404" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="AB11" s="12" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+      <c r="AB12" s="12" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>21</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>22</v>
+      </c>
+      <c r="AB13" s="12" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>435</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>367</v>
+      </c>
+      <c r="AB14" s="12" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AB15" s="12" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AB16" s="12" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="17" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB17" s="12" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="18" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB18" s="12" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="19" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB19" s="12" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="20" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB20" s="12" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="21" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB21" s="12" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="22" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB22" s="12" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="23" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB23" s="12" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="24" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB24" s="12" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="25" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB25" s="12" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="26" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB26" s="12" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="27" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB27" s="12" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="28" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB28" s="12" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="29" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB29" s="12" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="30" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB30" s="12" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="31" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB31" s="12" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="32" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB32" s="12" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="33" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB33" s="12" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="34" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB34" s="12" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="35" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB35" s="12" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="36" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB36" s="12" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="37" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB37" s="12" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="38" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB38" s="12" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="39" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB39" s="12" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="40" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB40" s="12" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="41" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB41" s="12" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="42" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB42" s="12" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="43" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB43" s="12" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="44" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB44" s="12" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="45" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB45" s="12" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="46" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB46" s="12" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="47" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB47" s="12" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="48" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB48" s="12" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="49" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB49" s="12" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="50" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB50" s="12" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="51" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB51" s="12" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="52" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB52" s="12" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="53" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB53" s="12" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="54" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB54" s="12" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="55" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB55" s="12" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="56" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB56" s="12" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="57" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB57" s="12" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="58" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB58" s="12" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="59" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB59" s="12" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="60" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB60" s="12" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="61" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB61" s="12" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="62" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB62" s="12" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="63" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB63" s="12" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="64" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB64" s="12" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="65" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB65" s="12" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="66" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB66" s="12" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="67" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB67" s="12" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="68" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB68" s="12" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="69" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB69" s="12" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="70" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB70" s="12" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="71" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB71" s="12" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="72" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB72" s="12" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="73" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB73" s="12" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="74" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB74" s="12" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="75" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB75" s="12" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="76" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB76" s="12" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="77" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB77" s="12" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="78" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB78" s="12" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="79" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB79" s="12" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="80" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB80" s="12" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="81" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB81" s="12" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="82" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB82" s="12" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="83" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB83" s="12" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="84" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB84" s="12" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="85" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB85" s="12" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="86" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB86" s="12" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="87" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB87" s="12" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="88" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB88" s="12" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="89" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB89" s="12" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="90" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB90" s="12" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="91" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB91" s="12" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="92" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB92" s="12" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="93" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB93" s="12" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="94" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB94" s="12" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="95" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB95" s="12" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="96" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB96" s="12" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="97" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB97" s="12" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="98" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB98" s="12" t="s">
+        <v>434</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>
   </mergeCells>
-  <dataValidations count="1">
+  <dataValidations count="2">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B8" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"-,All Categories,Backup and Disaster Recovery,Cloud Services,Communication and Collaboration,Customer Management,Digital Marketing,Finance,Human Resources,Infrastructure,IT Management,Marketing,Office Productivity,Sales,Security"</formula1>
+    </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B14" xr:uid="{E6E5BBA1-B8BB-434D-8671-C49E523C326B}">
+      <formula1>$AB$2:$AB$98</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2731,8 +3512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3134AC6-DDEE-044F-825B-D4DF0F5E2D02}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:E4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
LITE-23292 Add additional sheet for list of translations of the product
</commit_message>
<xml_diff>
--- a/tests/fixtures/comparation_product.xlsx
+++ b/tests/fixtures/comparation_product.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carlosherrero/projects/connect-cli/tests/fixtures/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jpaul00/cloud-blue-github/connect-cli/tests/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E12F042C-4FCA-6B48-9E1E-D06C0AAD913E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6163D4CD-2EA5-9041-9036-4FA45A78BFAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18720" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General Information" sheetId="1" r:id="rId1"/>
@@ -24,13 +24,14 @@
     <sheet name="Configuration Parameters" sheetId="15" r:id="rId9"/>
     <sheet name="Actions" sheetId="10" r:id="rId10"/>
     <sheet name="Configuration" sheetId="11" r:id="rId11"/>
+    <sheet name="Translations" sheetId="17" r:id="rId12"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="436">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="960" uniqueCount="450">
   <si>
     <t>Product information</t>
   </si>
@@ -1480,6 +1481,48 @@
   </si>
   <si>
     <t>Primary Translation Locale</t>
+  </si>
+  <si>
+    <t>Translation ID</t>
+  </si>
+  <si>
+    <t>Context</t>
+  </si>
+  <si>
+    <t>Owner ID</t>
+  </si>
+  <si>
+    <t>Owner</t>
+  </si>
+  <si>
+    <t>Locale</t>
+  </si>
+  <si>
+    <t>Autotranslation</t>
+  </si>
+  <si>
+    <t>Completion</t>
+  </si>
+  <si>
+    <t>Updated</t>
+  </si>
+  <si>
+    <t>inactive</t>
+  </si>
+  <si>
+    <t>TRN-1079-0833-9890</t>
+  </si>
+  <si>
+    <t>Persian</t>
+  </si>
+  <si>
+    <t>2020-10-15T01:19:20+00:00</t>
+  </si>
+  <si>
+    <t>2020-10-14T12:11:24+00:00</t>
+  </si>
+  <si>
+    <t>Context ID</t>
   </si>
 </sst>
 </file>
@@ -1548,7 +1591,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1571,6 +1614,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1879,7 +1924,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+    <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
@@ -1890,10 +1935,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="31" x14ac:dyDescent="0.2">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
+      <c r="B1" s="17"/>
       <c r="AB1" s="12" t="s">
         <v>337</v>
       </c>
@@ -3144,6 +3189,119 @@
   <dataValidations count="1">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D2:D19" xr:uid="{00000000-0002-0000-0A00-000000000000}">
       <formula1>"-,create,update,delete"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62DD5574-F1F3-8943-BAA8-7E6A93E385BA}">
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="5" width="25" style="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30" style="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="25" style="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="15" style="14" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="25" style="14" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.83203125" style="14"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>436</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>449</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>437</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>438</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>439</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>440</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>441</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>442</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="14" t="s">
+        <v>445</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>446</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2" s="15">
+        <v>1</v>
+      </c>
+      <c r="K2" s="14" t="s">
+        <v>444</v>
+      </c>
+      <c r="L2" s="14" t="s">
+        <v>448</v>
+      </c>
+      <c r="M2" s="14" t="s">
+        <v>447</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="I2" xr:uid="{9A8C9F8E-DBF7-EC4B-B398-272936245A56}">
+      <formula1>"Disabled,Enabled"</formula1>
+    </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{B4FC5392-A756-F544-921C-0A83426FE2C0}">
+      <formula1>"-,delete,update,create"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
[HF] LITE-23292 Add additional sheet for list of translations of the product
</commit_message>
<xml_diff>
--- a/tests/fixtures/comparation_product.xlsx
+++ b/tests/fixtures/comparation_product.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carlosherrero/projects/connect-cli/tests/fixtures/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jpaul00/cloud-blue-github/connect-cli/tests/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E12F042C-4FCA-6B48-9E1E-D06C0AAD913E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF9F0B5A-0C23-9240-9F35-A60F50C3CDE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18720" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General Information" sheetId="1" r:id="rId1"/>
@@ -24,13 +24,14 @@
     <sheet name="Configuration Parameters" sheetId="15" r:id="rId9"/>
     <sheet name="Actions" sheetId="10" r:id="rId10"/>
     <sheet name="Configuration" sheetId="11" r:id="rId11"/>
+    <sheet name="Translations" sheetId="16" r:id="rId12"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="436">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="960" uniqueCount="450">
   <si>
     <t>Product information</t>
   </si>
@@ -1480,6 +1481,48 @@
   </si>
   <si>
     <t>Primary Translation Locale</t>
+  </si>
+  <si>
+    <t>Translation ID</t>
+  </si>
+  <si>
+    <t>Context</t>
+  </si>
+  <si>
+    <t>Owner ID</t>
+  </si>
+  <si>
+    <t>Owner</t>
+  </si>
+  <si>
+    <t>Locale</t>
+  </si>
+  <si>
+    <t>Autotranslation</t>
+  </si>
+  <si>
+    <t>Completion</t>
+  </si>
+  <si>
+    <t>Updated</t>
+  </si>
+  <si>
+    <t>inactive</t>
+  </si>
+  <si>
+    <t>TRN-1079-0833-9890</t>
+  </si>
+  <si>
+    <t>Persian</t>
+  </si>
+  <si>
+    <t>2020-10-15T01:19:20+00:00</t>
+  </si>
+  <si>
+    <t>2020-10-14T12:11:24+00:00</t>
+  </si>
+  <si>
+    <t>Context ID</t>
   </si>
 </sst>
 </file>
@@ -1548,7 +1591,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1571,6 +1614,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1879,8 +1924,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1890,10 +1935,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="31" x14ac:dyDescent="0.2">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
+      <c r="B1" s="17"/>
       <c r="AB1" s="12" t="s">
         <v>337</v>
       </c>
@@ -3144,6 +3189,119 @@
   <dataValidations count="1">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D2:D19" xr:uid="{00000000-0002-0000-0A00-000000000000}">
       <formula1>"-,create,update,delete"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A975D84-394D-0140-B515-443DCD7E6E85}">
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="5" width="25" style="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30" style="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="25" style="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="15" style="14" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="25" style="14" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.83203125" style="14"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>436</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>449</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>437</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>438</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>439</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>440</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>441</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>442</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="14" t="s">
+        <v>445</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>446</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2" s="15">
+        <v>1</v>
+      </c>
+      <c r="K2" s="14" t="s">
+        <v>444</v>
+      </c>
+      <c r="L2" s="14" t="s">
+        <v>448</v>
+      </c>
+      <c r="M2" s="14" t="s">
+        <v>447</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="I2" xr:uid="{D7D560EC-DCE4-BF47-8293-5C924A86E41B}">
+      <formula1>"Disabled,Enabled"</formula1>
+    </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{17F0E032-D2C2-684A-B452-DF755A9E3D6D}">
+      <formula1>"-,delete,update,create"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
LITE-23293 Support of translation attributes inside xlsx file when user export the product
</commit_message>
<xml_diff>
--- a/tests/fixtures/comparation_product.xlsx
+++ b/tests/fixtures/comparation_product.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jpaul00/cloud-blue-github/connect-cli/tests/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6163D4CD-2EA5-9041-9036-4FA45A78BFAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05ED1984-761A-A249-9A29-63D8E07CA6FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18720" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18720" firstSheet="1" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General Information" sheetId="1" r:id="rId1"/>
@@ -25,13 +25,17 @@
     <sheet name="Actions" sheetId="10" r:id="rId10"/>
     <sheet name="Configuration" sheetId="11" r:id="rId11"/>
     <sheet name="Translations" sheetId="17" r:id="rId12"/>
+    <sheet name="TRN-1079-0833-9890 (FA)" sheetId="18" r:id="rId13"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">'TRN-1079-0833-9890 (FA)'!$A:$E</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="960" uniqueCount="450">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1065" uniqueCount="503">
   <si>
     <t>Product information</t>
   </si>
@@ -1524,12 +1528,189 @@
   <si>
     <t>Context ID</t>
   </si>
+  <si>
+    <t>Título del parámetro B</t>
+  </si>
+  <si>
+    <t>product.PRD-746-555-769.parameters.PRM-746-555-769-0002.title</t>
+  </si>
+  <si>
+    <t>otro valor</t>
+  </si>
+  <si>
+    <t>product.PRD-746-555-769.parameters.PRM-746-555-769-0002.placeholder</t>
+  </si>
+  <si>
+    <t>Esta es otra sola línea de texto</t>
+  </si>
+  <si>
+    <t>product.PRD-746-555-769.parameters.PRM-746-555-769-0002.hint</t>
+  </si>
+  <si>
+    <t>Descripción del parámetro B</t>
+  </si>
+  <si>
+    <t>product.PRD-746-555-769.parameters.PRM-746-555-769-0002.description</t>
+  </si>
+  <si>
+    <t>Título del parámetro A</t>
+  </si>
+  <si>
+    <t>product.PRD-746-555-769.parameters.PRM-746-555-769-0001.title</t>
+  </si>
+  <si>
+    <t>Escriba el valor del parámetro</t>
+  </si>
+  <si>
+    <t>product.PRD-746-555-769.parameters.PRM-746-555-769-0001.placeholder</t>
+  </si>
+  <si>
+    <t>Se trata de una sola línea de texto</t>
+  </si>
+  <si>
+    <t>product.PRD-746-555-769.parameters.PRM-746-555-769-0001.hint</t>
+  </si>
+  <si>
+    <t>Descripción del parámetro A</t>
+  </si>
+  <si>
+    <t>product.PRD-746-555-769.parameters.PRM-746-555-769-0001.description</t>
+  </si>
+  <si>
+    <t>producto de prueba para traducciones</t>
+  </si>
+  <si>
+    <t>product.PRD-746-555-769.name</t>
+  </si>
+  <si>
+    <t>Prd 746 555 769 0002</t>
+  </si>
+  <si>
+    <t>product.PRD-746-555-769.items.PRD-746-555-769-0002.name</t>
+  </si>
+  <si>
+    <t>MPN-B</t>
+  </si>
+  <si>
+    <t>product.PRD-746-555-769.items.PRD-746-555-769-0002.description</t>
+  </si>
+  <si>
+    <t>Prd 746 555 769 0001</t>
+  </si>
+  <si>
+    <t>product.PRD-746-555-769.items.PRD-746-555-769-0001.name</t>
+  </si>
+  <si>
+    <t>MPN-A</t>
+  </si>
+  <si>
+    <t>product.PRD-746-555-769.items.PRD-746-555-769-0001.description</t>
+  </si>
+  <si>
+    <t>Un texto **descripción** del producto. Este texto será visto por los proveedores que tienen acceso a este producto y se puede utilizar para rellenar otros sistemas, como [CloudBlue Catalog](https://catalog.cloudblue.com).
+La **primera oración** (alrededor de 3-4 líneas) de esta descripción **cuenta más**. Por lo tanto, comience con una oración que llame la atención y que presente claramente a los usuarios para qué está destinado el producto.
+Tenga en cuenta las siguientes recomendaciones con respecto a la descripción del producto:
+* Manténgalo conciso, informativo y fácil de entender
+* Apégate al tono de tu marca
+* Evite términos específicos, manténgalo simple
+* Asegúrese de describir el público objetivo de este producto
+* Esbozar características clave y diferenciadores clave
+Tenga en cuenta que el espacio máximo permitido es de ** hasta 4,000 caracteres ** - asegúrese de explicar su producto dentro de ese límite.
+# Usar texto con formato
+CloudBlue Connect le permite enriquecer esta descripción con el formato [texto de marcado](https://en.wikipedia.org/wiki/Markdown). **Markdown** permite incluir múltiples elementos, como* Listas de elementos sin ordenar, como esta
+* Listas ordenadas, como la siguiente
+    1. Primer punto
+    2. Segundo punto
+* Estilos de fuente, como *italic*, **bold** y 'monospace'
+* Encabezados: tenga en cuenta que recomendamos encarecidamente usar solo ## para este documento
+# Para más información
+Consulte nuestra **[documentación](https://connect.cloudblue.com/documentation)** para obtener más información sobre las capacidades del editor de productos.
+## ELIMINE ESTE TEXTO ANTES DE PUBLICAR SU PRODUCTO.</t>
+  </si>
+  <si>
+    <t>product.PRD-746-555-769.detailed_overview</t>
+  </si>
+  <si>
+    <t>Descripción corta del producto.</t>
+  </si>
+  <si>
+    <t>product.PRD-746-555-769.description</t>
+  </si>
+  <si>
+    <t>Por favor, espere mientras se cumple su solicitud.</t>
+  </si>
+  <si>
+    <t>product.PRD-746-555-769.customer_ui_settings.provisioning_message</t>
+  </si>
+  <si>
+    <t>Ahora está listo para usar el servicio en la nube y migrar los archivos desde su equipo local y dispositivos móviles a la nube. Descargue aplicaciones para Windows Desktop, Windows Phone, Mac OS o Android siguiendo uno de los siguientes enlaces, o acceda directamente a la interfaz web del servicio.</t>
+  </si>
+  <si>
+    <t>product.PRD-746-555-769.customer_ui_settings.getting_started</t>
+  </si>
+  <si>
+    <t>product.PRD-746-555-769.customer_ui_settings.download_links.3.url</t>
+  </si>
+  <si>
+    <t>product.PRD-746-555-769.customer_ui_settings.download_links.3.title</t>
+  </si>
+  <si>
+    <t>product.PRD-746-555-769.customer_ui_settings.download_links.2.url</t>
+  </si>
+  <si>
+    <t>product.PRD-746-555-769.customer_ui_settings.download_links.2.title</t>
+  </si>
+  <si>
+    <t>product.PRD-746-555-769.customer_ui_settings.download_links.1.url</t>
+  </si>
+  <si>
+    <t>product.PRD-746-555-769.customer_ui_settings.download_links.1.title</t>
+  </si>
+  <si>
+    <t>product.PRD-746-555-769.customer_ui_settings.download_links.0.url</t>
+  </si>
+  <si>
+    <t>product.PRD-746-555-769.customer_ui_settings.download_links.0.title</t>
+  </si>
+  <si>
+    <t>product.PRD-746-555-769.customer_ui_settings.documents.0.url</t>
+  </si>
+  <si>
+    <t>product.PRD-746-555-769.customer_ui_settings.documents.0.title</t>
+  </si>
+  <si>
+    <t>Nos complace proporcionarle el servicio en la nube, una solución definitiva para su empresa. Deje de usar la solución local heredada en el equipo. Muévase a la nube con nuestra ayuda.</t>
+  </si>
+  <si>
+    <t>product.PRD-746-555-769.customer_ui_settings.description</t>
+  </si>
+  <si>
+    <t>Inicia sesión</t>
+  </si>
+  <si>
+    <t>product.PRD-746-555-769.actions.ACT-746-555-769-001.name</t>
+  </si>
+  <si>
+    <t>Inicie sesión en el servicio haciendo clic en este botón</t>
+  </si>
+  <si>
+    <t>product.PRD-746-555-769.actions.ACT-746-555-769-001.description</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Original Value</t>
+  </si>
+  <si>
+    <t>Key</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1560,8 +1741,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1578,6 +1765,11 @@
         <fgColor rgb="FFD3D3D3"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFAEAEAE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1591,7 +1783,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1616,10 +1808,21 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1935,10 +2138,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="31" x14ac:dyDescent="0.2">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
+      <c r="B1" s="18"/>
       <c r="AB1" s="12" t="s">
         <v>337</v>
       </c>
@@ -3199,7 +3402,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62DD5574-F1F3-8943-BAA8-7E6A93E385BA}">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
@@ -3302,6 +3505,432 @@
     </dataValidation>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{B4FC5392-A756-F544-921C-0A83426FE2C0}">
       <formula1>"-,delete,update,create"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37EF1FCC-8CBB-134E-BA5D-137ED4CA26F7}">
+  <dimension ref="A1:E31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="100" style="16" customWidth="1"/>
+    <col min="3" max="3" width="20" style="16" customWidth="1"/>
+    <col min="4" max="4" width="100" style="16" customWidth="1"/>
+    <col min="5" max="5" width="30" style="16" customWidth="1"/>
+    <col min="6" max="16384" width="8.83203125" style="16"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="20" t="s">
+        <v>502</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>501</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="16" t="s">
+        <v>499</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>498</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="16" t="s">
+        <v>497</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>496</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A4" s="16" t="s">
+        <v>495</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>494</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="16" t="s">
+        <v>493</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="5"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="16" t="s">
+        <v>492</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="5"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="16" t="s">
+        <v>491</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="5"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="16" t="s">
+        <v>490</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="5"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="16" t="s">
+        <v>489</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="5"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="16" t="s">
+        <v>488</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="5"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="16" t="s">
+        <v>487</v>
+      </c>
+      <c r="B11" s="5"/>
+      <c r="C11" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="5"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="5"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="16" t="s">
+        <v>485</v>
+      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="5"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="16" t="s">
+        <v>484</v>
+      </c>
+      <c r="B14" s="5"/>
+      <c r="C14" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="5"/>
+    </row>
+    <row r="15" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="A15" s="16" t="s">
+        <v>483</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>482</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="16" t="s">
+        <v>481</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>480</v>
+      </c>
+      <c r="C16" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" s="16" t="s">
+        <v>479</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>478</v>
+      </c>
+      <c r="C17" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A18" s="16" t="s">
+        <v>477</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>476</v>
+      </c>
+      <c r="C18" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" s="16" t="s">
+        <v>475</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>474</v>
+      </c>
+      <c r="C19" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A20" s="16" t="s">
+        <v>473</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>472</v>
+      </c>
+      <c r="C20" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" s="16" t="s">
+        <v>471</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>470</v>
+      </c>
+      <c r="C21" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" s="16" t="s">
+        <v>469</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>468</v>
+      </c>
+      <c r="C22" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A23" s="16" t="s">
+        <v>467</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>466</v>
+      </c>
+      <c r="C23" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24" s="16" t="s">
+        <v>465</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>464</v>
+      </c>
+      <c r="C24" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A25" s="16" t="s">
+        <v>463</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>462</v>
+      </c>
+      <c r="C25" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A26" s="16" t="s">
+        <v>461</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>460</v>
+      </c>
+      <c r="C26" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A27" s="16" t="s">
+        <v>459</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>458</v>
+      </c>
+      <c r="C27" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A28" s="16" t="s">
+        <v>457</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>456</v>
+      </c>
+      <c r="C28" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A29" s="16" t="s">
+        <v>455</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>454</v>
+      </c>
+      <c r="C29" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A30" s="16" t="s">
+        <v>453</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>452</v>
+      </c>
+      <c r="C30" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A31" s="16" t="s">
+        <v>451</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>450</v>
+      </c>
+      <c r="C31" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>450</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:E1048576" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
+  <dataValidations count="1">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C31" xr:uid="{41F776B4-F1F5-E449-BA83-3EB23C2095AB}">
+      <formula1>"-,update"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Fix translation attributes sheet headers when export to xlsx
</commit_message>
<xml_diff>
--- a/tests/fixtures/comparation_product.xlsx
+++ b/tests/fixtures/comparation_product.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jpaul00/cloud-blue-github/connect-cli/tests/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05ED1984-761A-A249-9A29-63D8E07CA6FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FE92284-143E-A64B-83E9-0266CB934A5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18720" firstSheet="1" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,17 +25,17 @@
     <sheet name="Actions" sheetId="10" r:id="rId10"/>
     <sheet name="Configuration" sheetId="11" r:id="rId11"/>
     <sheet name="Translations" sheetId="17" r:id="rId12"/>
-    <sheet name="TRN-1079-0833-9890 (FA)" sheetId="18" r:id="rId13"/>
+    <sheet name="FA (TRN-1079-0833-9890)" sheetId="18" r:id="rId13"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">'TRN-1079-0833-9890 (FA)'!$A:$E</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">'FA (TRN-1079-0833-9890)'!$A:$E</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1065" uniqueCount="503">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1096" uniqueCount="506">
   <si>
     <t>Product information</t>
   </si>
@@ -1697,13 +1697,22 @@
     <t>product.PRD-746-555-769.actions.ACT-746-555-769-001.description</t>
   </si>
   <si>
-    <t>Comment</t>
-  </si>
-  <si>
-    <t>Original Value</t>
-  </si>
-  <si>
-    <t>Key</t>
+    <t>Persian (TRN-1079-0833-9890)</t>
+  </si>
+  <si>
+    <t>key</t>
+  </si>
+  <si>
+    <t>action</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>editor</t>
   </si>
 </sst>
 </file>
@@ -1783,7 +1792,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1809,9 +1818,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1823,6 +1829,10 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2138,10 +2148,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="31" x14ac:dyDescent="0.2">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
+      <c r="B1" s="23"/>
       <c r="AB1" s="12" t="s">
         <v>337</v>
       </c>
@@ -3513,11 +3523,11 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37EF1FCC-8CBB-134E-BA5D-137ED4CA26F7}">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3529,401 +3539,494 @@
     <col min="6" max="16384" width="8.83203125" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="19" t="s">
+        <v>501</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>500</v>
+      </c>
+      <c r="C1" s="19" t="s">
         <v>502</v>
       </c>
-      <c r="B1" s="22" t="s">
-        <v>501</v>
-      </c>
-      <c r="C1" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" s="20" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="D1" s="20" t="s">
+        <v>503</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>504</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
         <v>499</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>498</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="18" t="s">
         <v>27</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>498</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="F2" s="16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="16" t="s">
         <v>497</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>496</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="18" t="s">
         <v>27</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>496</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="F3" s="17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>495</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>494</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="18" t="s">
         <v>27</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>494</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4" s="17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
         <v>493</v>
       </c>
       <c r="B5" s="5"/>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="18" t="s">
         <v>27</v>
       </c>
       <c r="D5" s="5"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5" s="17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="16" t="s">
         <v>492</v>
       </c>
       <c r="B6" s="5"/>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="18" t="s">
         <v>27</v>
       </c>
       <c r="D6" s="5"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F6" s="17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="16" t="s">
         <v>491</v>
       </c>
       <c r="B7" s="5"/>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="18" t="s">
         <v>27</v>
       </c>
       <c r="D7" s="5"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F7" s="17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="16" t="s">
         <v>490</v>
       </c>
       <c r="B8" s="5"/>
-      <c r="C8" s="19" t="s">
+      <c r="C8" s="18" t="s">
         <v>27</v>
       </c>
       <c r="D8" s="5"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F8" s="17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="16" t="s">
         <v>489</v>
       </c>
       <c r="B9" s="5"/>
-      <c r="C9" s="19" t="s">
+      <c r="C9" s="18" t="s">
         <v>27</v>
       </c>
       <c r="D9" s="5"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F9" s="17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
         <v>488</v>
       </c>
       <c r="B10" s="5"/>
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="18" t="s">
         <v>27</v>
       </c>
       <c r="D10" s="5"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F10" s="17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="16" t="s">
         <v>487</v>
       </c>
       <c r="B11" s="5"/>
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="18" t="s">
         <v>27</v>
       </c>
       <c r="D11" s="5"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F11" s="17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="16" t="s">
         <v>486</v>
       </c>
       <c r="B12" s="5"/>
-      <c r="C12" s="19" t="s">
+      <c r="C12" s="18" t="s">
         <v>27</v>
       </c>
       <c r="D12" s="5"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F12" s="17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="16" t="s">
         <v>485</v>
       </c>
       <c r="B13" s="5"/>
-      <c r="C13" s="19" t="s">
+      <c r="C13" s="18" t="s">
         <v>27</v>
       </c>
       <c r="D13" s="5"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F13" s="17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>484</v>
       </c>
       <c r="B14" s="5"/>
-      <c r="C14" s="19" t="s">
+      <c r="C14" s="18" t="s">
         <v>27</v>
       </c>
       <c r="D14" s="5"/>
-    </row>
-    <row r="15" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="F14" s="17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A15" s="16" t="s">
         <v>483</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>482</v>
       </c>
-      <c r="C15" s="19" t="s">
+      <c r="C15" s="18" t="s">
         <v>27</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>482</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="F15" s="17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="16" t="s">
         <v>481</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="C16" s="19" t="s">
+      <c r="C16" s="18" t="s">
         <v>27</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>480</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="F16" s="17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="16" t="s">
         <v>479</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>478</v>
       </c>
-      <c r="C17" s="19" t="s">
+      <c r="C17" s="18" t="s">
         <v>27</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="F17" s="17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A18" s="16" t="s">
         <v>477</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>476</v>
       </c>
-      <c r="C18" s="19" t="s">
+      <c r="C18" s="18" t="s">
         <v>27</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>476</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="F18" s="17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="16" t="s">
         <v>475</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>474</v>
       </c>
-      <c r="C19" s="19" t="s">
+      <c r="C19" s="18" t="s">
         <v>27</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>474</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="F19" s="17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="16" t="s">
         <v>473</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>472</v>
       </c>
-      <c r="C20" s="19" t="s">
+      <c r="C20" s="18" t="s">
         <v>27</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>472</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="F20" s="17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="16" t="s">
         <v>471</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>470</v>
       </c>
-      <c r="C21" s="19" t="s">
+      <c r="C21" s="18" t="s">
         <v>27</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>470</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="F21" s="17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="16" t="s">
         <v>469</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>468</v>
       </c>
-      <c r="C22" s="19" t="s">
+      <c r="C22" s="18" t="s">
         <v>27</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>468</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="F22" s="17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="16" t="s">
         <v>467</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>466</v>
       </c>
-      <c r="C23" s="19" t="s">
+      <c r="C23" s="18" t="s">
         <v>27</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>466</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="F23" s="17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="16" t="s">
         <v>465</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>464</v>
       </c>
-      <c r="C24" s="19" t="s">
+      <c r="C24" s="18" t="s">
         <v>27</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>464</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="F24" s="17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="16" t="s">
         <v>463</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>462</v>
       </c>
-      <c r="C25" s="19" t="s">
+      <c r="C25" s="18" t="s">
         <v>27</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="F25" s="17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="16" t="s">
         <v>461</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>460</v>
       </c>
-      <c r="C26" s="19" t="s">
+      <c r="C26" s="18" t="s">
         <v>27</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>460</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="F26" s="17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="16" t="s">
         <v>459</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>458</v>
       </c>
-      <c r="C27" s="19" t="s">
+      <c r="C27" s="18" t="s">
         <v>27</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="F27" s="17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="16" t="s">
         <v>457</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>456</v>
       </c>
-      <c r="C28" s="19" t="s">
+      <c r="C28" s="18" t="s">
         <v>27</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="F28" s="17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="16" t="s">
         <v>455</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>454</v>
       </c>
-      <c r="C29" s="19" t="s">
+      <c r="C29" s="18" t="s">
         <v>27</v>
       </c>
       <c r="D29" s="5" t="s">
         <v>454</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="F29" s="17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="16" t="s">
         <v>453</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>452</v>
       </c>
-      <c r="C30" s="19" t="s">
+      <c r="C30" s="18" t="s">
         <v>27</v>
       </c>
       <c r="D30" s="5" t="s">
         <v>452</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="F30" s="17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="16" t="s">
         <v>451</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>450</v>
       </c>
-      <c r="C31" s="19" t="s">
+      <c r="C31" s="18" t="s">
         <v>27</v>
       </c>
       <c r="D31" s="5" t="s">
         <v>450</v>
+      </c>
+      <c r="F31" s="17" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
LITE-23295: validate translations in product sync
</commit_message>
<xml_diff>
--- a/tests/fixtures/comparation_product.xlsx
+++ b/tests/fixtures/comparation_product.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jpaul00/cloud-blue-github/connect-cli/tests/fixtures/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carlosherrero/projects/connect-cli/tests/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FE92284-143E-A64B-83E9-0266CB934A5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D361EFA0-7363-0046-BB5F-6DD5B3ACF7DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18720" firstSheet="1" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" firstSheet="3" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General Information" sheetId="1" r:id="rId1"/>
@@ -25,17 +25,14 @@
     <sheet name="Actions" sheetId="10" r:id="rId10"/>
     <sheet name="Configuration" sheetId="11" r:id="rId11"/>
     <sheet name="Translations" sheetId="17" r:id="rId12"/>
-    <sheet name="FA (TRN-1079-0833-9890)" sheetId="18" r:id="rId13"/>
+    <sheet name="FA (TRN-1079-0833-9890)" sheetId="19" r:id="rId13"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">'FA (TRN-1079-0833-9890)'!$A:$E</definedName>
-  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1096" uniqueCount="506">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1098" uniqueCount="507">
   <si>
     <t>Product information</t>
   </si>
@@ -1517,9 +1514,6 @@
     <t>TRN-1079-0833-9890</t>
   </si>
   <si>
-    <t>Persian</t>
-  </si>
-  <si>
     <t>2020-10-15T01:19:20+00:00</t>
   </si>
   <si>
@@ -1697,10 +1691,16 @@
     <t>product.PRD-746-555-769.actions.ACT-746-555-769-001.description</t>
   </si>
   <si>
+    <t>Is primary</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>key</t>
+  </si>
+  <si>
     <t>Persian (TRN-1079-0833-9890)</t>
-  </si>
-  <si>
-    <t>key</t>
   </si>
   <si>
     <t>action</t>
@@ -1818,7 +1818,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1829,6 +1828,7 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2137,8 +2137,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB98"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3410,10 +3410,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62DD5574-F1F3-8943-BAA8-7E6A93E385BA}">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3422,11 +3422,12 @@
     <col min="6" max="6" width="30" style="14" bestFit="1" customWidth="1"/>
     <col min="7" max="9" width="25" style="14" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="15" style="14" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="25" style="14" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.83203125" style="14"/>
+    <col min="12" max="12" width="15" style="16" customWidth="1"/>
+    <col min="13" max="14" width="25" style="14" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="8.83203125" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>436</v>
       </c>
@@ -3434,7 +3435,7 @@
         <v>24</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>437</v>
@@ -3461,13 +3462,16 @@
         <v>88</v>
       </c>
       <c r="L1" s="6" t="s">
+        <v>499</v>
+      </c>
+      <c r="M1" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
         <v>445</v>
       </c>
@@ -3486,8 +3490,8 @@
       <c r="F2" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="14" t="s">
-        <v>446</v>
+      <c r="G2" s="13" t="s">
+        <v>367</v>
       </c>
       <c r="H2" s="5" t="s">
         <v>27</v>
@@ -3501,11 +3505,14 @@
       <c r="K2" s="14" t="s">
         <v>444</v>
       </c>
-      <c r="L2" s="14" t="s">
-        <v>448</v>
+      <c r="L2" s="16" t="s">
+        <v>500</v>
       </c>
       <c r="M2" s="14" t="s">
         <v>447</v>
+      </c>
+      <c r="N2" s="14" t="s">
+        <v>446</v>
       </c>
     </row>
   </sheetData>
@@ -3518,525 +3525,535 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{6432594F-761A-6946-AEAF-FEF01186A0B2}">
+          <x14:formula1>
+            <xm:f>'General Information'!$AB$2:$AB$98</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37EF1FCC-8CBB-134E-BA5D-137ED4CA26F7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21A7B334-F5B6-C244-A533-FEB6F9AB5CB8}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="100" style="16" customWidth="1"/>
-    <col min="3" max="3" width="20" style="16" customWidth="1"/>
-    <col min="4" max="4" width="100" style="16" customWidth="1"/>
-    <col min="5" max="5" width="30" style="16" customWidth="1"/>
-    <col min="6" max="16384" width="8.83203125" style="16"/>
+    <col min="1" max="2" width="100" style="21" customWidth="1"/>
+    <col min="3" max="3" width="20" style="21" customWidth="1"/>
+    <col min="4" max="4" width="100" style="21" customWidth="1"/>
+    <col min="5" max="5" width="30" style="21" customWidth="1"/>
+    <col min="6" max="16384" width="8.83203125" style="21"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="18" t="s">
         <v>501</v>
       </c>
-      <c r="B1" s="21" t="s">
-        <v>500</v>
-      </c>
-      <c r="C1" s="19" t="s">
+      <c r="B1" s="20" t="s">
         <v>502</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="C1" s="18" t="s">
         <v>503</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="D1" s="19" t="s">
         <v>504</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="E1" s="18" t="s">
         <v>505</v>
       </c>
+      <c r="F1" s="18" t="s">
+        <v>506</v>
+      </c>
     </row>
     <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="16" t="s">
-        <v>499</v>
+      <c r="A2" s="21" t="s">
+        <v>498</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>498</v>
-      </c>
-      <c r="C2" s="18" t="s">
+        <v>497</v>
+      </c>
+      <c r="C2" s="17" t="s">
         <v>27</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>498</v>
-      </c>
-      <c r="F2" s="16" t="s">
+        <v>497</v>
+      </c>
+      <c r="F2" s="21" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="16" t="s">
-        <v>497</v>
+      <c r="A3" s="21" t="s">
+        <v>496</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>496</v>
-      </c>
-      <c r="C3" s="18" t="s">
+        <v>495</v>
+      </c>
+      <c r="C3" s="17" t="s">
         <v>27</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>496</v>
-      </c>
-      <c r="F3" s="17" t="s">
+        <v>495</v>
+      </c>
+      <c r="F3" s="21" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A4" s="16" t="s">
-        <v>495</v>
+      <c r="A4" s="21" t="s">
+        <v>494</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>494</v>
-      </c>
-      <c r="C4" s="18" t="s">
+        <v>493</v>
+      </c>
+      <c r="C4" s="17" t="s">
         <v>27</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>494</v>
-      </c>
-      <c r="F4" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="F4" s="21" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="16" t="s">
-        <v>493</v>
+      <c r="A5" s="21" t="s">
+        <v>492</v>
       </c>
       <c r="B5" s="5"/>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="17" t="s">
         <v>27</v>
       </c>
       <c r="D5" s="5"/>
-      <c r="F5" s="17" t="s">
+      <c r="F5" s="21" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="16" t="s">
-        <v>492</v>
+      <c r="A6" s="21" t="s">
+        <v>491</v>
       </c>
       <c r="B6" s="5"/>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="17" t="s">
         <v>27</v>
       </c>
       <c r="D6" s="5"/>
-      <c r="F6" s="17" t="s">
+      <c r="F6" s="21" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="16" t="s">
-        <v>491</v>
+      <c r="A7" s="21" t="s">
+        <v>490</v>
       </c>
       <c r="B7" s="5"/>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="17" t="s">
         <v>27</v>
       </c>
       <c r="D7" s="5"/>
-      <c r="F7" s="17" t="s">
+      <c r="F7" s="21" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="16" t="s">
-        <v>490</v>
+      <c r="A8" s="21" t="s">
+        <v>489</v>
       </c>
       <c r="B8" s="5"/>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="17" t="s">
         <v>27</v>
       </c>
       <c r="D8" s="5"/>
-      <c r="F8" s="17" t="s">
+      <c r="F8" s="21" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="16" t="s">
-        <v>489</v>
+      <c r="A9" s="21" t="s">
+        <v>488</v>
       </c>
       <c r="B9" s="5"/>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="17" t="s">
         <v>27</v>
       </c>
       <c r="D9" s="5"/>
-      <c r="F9" s="17" t="s">
+      <c r="F9" s="21" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="16" t="s">
-        <v>488</v>
+      <c r="A10" s="21" t="s">
+        <v>487</v>
       </c>
       <c r="B10" s="5"/>
-      <c r="C10" s="18" t="s">
+      <c r="C10" s="17" t="s">
         <v>27</v>
       </c>
       <c r="D10" s="5"/>
-      <c r="F10" s="17" t="s">
+      <c r="F10" s="21" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="16" t="s">
-        <v>487</v>
+      <c r="A11" s="21" t="s">
+        <v>486</v>
       </c>
       <c r="B11" s="5"/>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="17" t="s">
         <v>27</v>
       </c>
       <c r="D11" s="5"/>
-      <c r="F11" s="17" t="s">
+      <c r="F11" s="21" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="16" t="s">
-        <v>486</v>
+      <c r="A12" s="21" t="s">
+        <v>485</v>
       </c>
       <c r="B12" s="5"/>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="17" t="s">
         <v>27</v>
       </c>
       <c r="D12" s="5"/>
-      <c r="F12" s="17" t="s">
+      <c r="F12" s="21" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="16" t="s">
-        <v>485</v>
+      <c r="A13" s="21" t="s">
+        <v>484</v>
       </c>
       <c r="B13" s="5"/>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="17" t="s">
         <v>27</v>
       </c>
       <c r="D13" s="5"/>
-      <c r="F13" s="17" t="s">
+      <c r="F13" s="21" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="16" t="s">
-        <v>484</v>
+      <c r="A14" s="21" t="s">
+        <v>483</v>
       </c>
       <c r="B14" s="5"/>
-      <c r="C14" s="18" t="s">
+      <c r="C14" s="17" t="s">
         <v>27</v>
       </c>
       <c r="D14" s="5"/>
-      <c r="F14" s="17" t="s">
+      <c r="F14" s="21" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A15" s="16" t="s">
-        <v>483</v>
+      <c r="A15" s="21" t="s">
+        <v>482</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>482</v>
-      </c>
-      <c r="C15" s="18" t="s">
+        <v>481</v>
+      </c>
+      <c r="C15" s="17" t="s">
         <v>27</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>482</v>
-      </c>
-      <c r="F15" s="17" t="s">
+        <v>481</v>
+      </c>
+      <c r="F15" s="21" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="16" t="s">
-        <v>481</v>
+      <c r="A16" s="21" t="s">
+        <v>480</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>480</v>
-      </c>
-      <c r="C16" s="18" t="s">
+        <v>479</v>
+      </c>
+      <c r="C16" s="17" t="s">
         <v>27</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>480</v>
-      </c>
-      <c r="F16" s="17" t="s">
+        <v>479</v>
+      </c>
+      <c r="F16" s="21" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A17" s="16" t="s">
-        <v>479</v>
+      <c r="A17" s="21" t="s">
+        <v>478</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>478</v>
-      </c>
-      <c r="C17" s="18" t="s">
+        <v>477</v>
+      </c>
+      <c r="C17" s="17" t="s">
         <v>27</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>478</v>
-      </c>
-      <c r="F17" s="17" t="s">
+        <v>477</v>
+      </c>
+      <c r="F17" s="21" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A18" s="16" t="s">
-        <v>477</v>
+      <c r="A18" s="21" t="s">
+        <v>476</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>476</v>
-      </c>
-      <c r="C18" s="18" t="s">
+        <v>475</v>
+      </c>
+      <c r="C18" s="17" t="s">
         <v>27</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>476</v>
-      </c>
-      <c r="F18" s="17" t="s">
+        <v>475</v>
+      </c>
+      <c r="F18" s="21" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A19" s="16" t="s">
-        <v>475</v>
+      <c r="A19" s="21" t="s">
+        <v>474</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>474</v>
-      </c>
-      <c r="C19" s="18" t="s">
+        <v>473</v>
+      </c>
+      <c r="C19" s="17" t="s">
         <v>27</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>474</v>
-      </c>
-      <c r="F19" s="17" t="s">
+        <v>473</v>
+      </c>
+      <c r="F19" s="21" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A20" s="16" t="s">
-        <v>473</v>
+      <c r="A20" s="21" t="s">
+        <v>472</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>472</v>
-      </c>
-      <c r="C20" s="18" t="s">
+        <v>471</v>
+      </c>
+      <c r="C20" s="17" t="s">
         <v>27</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>472</v>
-      </c>
-      <c r="F20" s="17" t="s">
+        <v>471</v>
+      </c>
+      <c r="F20" s="21" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A21" s="16" t="s">
-        <v>471</v>
+      <c r="A21" s="21" t="s">
+        <v>470</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>470</v>
-      </c>
-      <c r="C21" s="18" t="s">
+        <v>469</v>
+      </c>
+      <c r="C21" s="17" t="s">
         <v>27</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>470</v>
-      </c>
-      <c r="F21" s="17" t="s">
+        <v>469</v>
+      </c>
+      <c r="F21" s="21" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A22" s="16" t="s">
-        <v>469</v>
+      <c r="A22" s="21" t="s">
+        <v>468</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>468</v>
-      </c>
-      <c r="C22" s="18" t="s">
+        <v>467</v>
+      </c>
+      <c r="C22" s="17" t="s">
         <v>27</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>468</v>
-      </c>
-      <c r="F22" s="17" t="s">
+        <v>467</v>
+      </c>
+      <c r="F22" s="21" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A23" s="16" t="s">
-        <v>467</v>
+      <c r="A23" s="21" t="s">
+        <v>466</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>466</v>
-      </c>
-      <c r="C23" s="18" t="s">
+        <v>465</v>
+      </c>
+      <c r="C23" s="17" t="s">
         <v>27</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>466</v>
-      </c>
-      <c r="F23" s="17" t="s">
+        <v>465</v>
+      </c>
+      <c r="F23" s="21" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A24" s="16" t="s">
-        <v>465</v>
+      <c r="A24" s="21" t="s">
+        <v>464</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>464</v>
-      </c>
-      <c r="C24" s="18" t="s">
+        <v>463</v>
+      </c>
+      <c r="C24" s="17" t="s">
         <v>27</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>464</v>
-      </c>
-      <c r="F24" s="17" t="s">
+        <v>463</v>
+      </c>
+      <c r="F24" s="21" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A25" s="16" t="s">
-        <v>463</v>
+      <c r="A25" s="21" t="s">
+        <v>462</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>462</v>
-      </c>
-      <c r="C25" s="18" t="s">
+        <v>461</v>
+      </c>
+      <c r="C25" s="17" t="s">
         <v>27</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>462</v>
-      </c>
-      <c r="F25" s="17" t="s">
+        <v>461</v>
+      </c>
+      <c r="F25" s="21" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A26" s="16" t="s">
-        <v>461</v>
+      <c r="A26" s="21" t="s">
+        <v>460</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>460</v>
-      </c>
-      <c r="C26" s="18" t="s">
+        <v>459</v>
+      </c>
+      <c r="C26" s="17" t="s">
         <v>27</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>460</v>
-      </c>
-      <c r="F26" s="17" t="s">
+        <v>459</v>
+      </c>
+      <c r="F26" s="21" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A27" s="16" t="s">
-        <v>459</v>
+      <c r="A27" s="21" t="s">
+        <v>458</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>458</v>
-      </c>
-      <c r="C27" s="18" t="s">
+        <v>457</v>
+      </c>
+      <c r="C27" s="17" t="s">
         <v>27</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>458</v>
-      </c>
-      <c r="F27" s="17" t="s">
+        <v>457</v>
+      </c>
+      <c r="F27" s="21" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A28" s="16" t="s">
-        <v>457</v>
+      <c r="A28" s="21" t="s">
+        <v>456</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>456</v>
-      </c>
-      <c r="C28" s="18" t="s">
+        <v>455</v>
+      </c>
+      <c r="C28" s="17" t="s">
         <v>27</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>456</v>
-      </c>
-      <c r="F28" s="17" t="s">
+        <v>455</v>
+      </c>
+      <c r="F28" s="21" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A29" s="16" t="s">
-        <v>455</v>
+      <c r="A29" s="21" t="s">
+        <v>454</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>454</v>
-      </c>
-      <c r="C29" s="18" t="s">
+        <v>453</v>
+      </c>
+      <c r="C29" s="17" t="s">
         <v>27</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>454</v>
-      </c>
-      <c r="F29" s="17" t="s">
+        <v>453</v>
+      </c>
+      <c r="F29" s="21" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A30" s="16" t="s">
-        <v>453</v>
+      <c r="A30" s="21" t="s">
+        <v>452</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>452</v>
-      </c>
-      <c r="C30" s="18" t="s">
+        <v>451</v>
+      </c>
+      <c r="C30" s="17" t="s">
         <v>27</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>452</v>
-      </c>
-      <c r="F30" s="17" t="s">
+        <v>451</v>
+      </c>
+      <c r="F30" s="21" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A31" s="16" t="s">
-        <v>451</v>
+      <c r="A31" s="21" t="s">
+        <v>450</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>450</v>
-      </c>
-      <c r="C31" s="18" t="s">
+        <v>449</v>
+      </c>
+      <c r="C31" s="17" t="s">
         <v>27</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>450</v>
-      </c>
-      <c r="F31" s="17" t="s">
+        <v>449</v>
+      </c>
+      <c r="F31" s="21" t="s">
         <v>27</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E1048576" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
   <dataValidations count="1">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C31" xr:uid="{41F776B4-F1F5-E449-BA83-3EB23C2095AB}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C31" xr:uid="{FEEBFAA0-9D60-894E-9FA3-F69C7A983591}">
       <formula1>"-,update"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
LITE-23296: sync product translations
Perform create/update/delete actions on the translations of the product.
(This does nothing on translation attributes)
</commit_message>
<xml_diff>
--- a/tests/fixtures/comparation_product.xlsx
+++ b/tests/fixtures/comparation_product.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carlosherrero/projects/connect-cli/tests/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D361EFA0-7363-0046-BB5F-6DD5B3ACF7DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EC4C238-7306-0641-9EFA-135853587078}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" firstSheet="3" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" firstSheet="3" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General Information" sheetId="1" r:id="rId1"/>
@@ -3412,8 +3412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62DD5574-F1F3-8943-BAA8-7E6A93E385BA}">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3521,7 +3521,7 @@
       <formula1>"Disabled,Enabled"</formula1>
     </dataValidation>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{B4FC5392-A756-F544-921C-0A83426FE2C0}">
-      <formula1>"-,delete,update,create"</formula1>
+      <formula1>"-"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3544,7 +3544,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21A7B334-F5B6-C244-A533-FEB6F9AB5CB8}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
LITE-23297: sync translation attributes on product sync
</commit_message>
<xml_diff>
--- a/tests/fixtures/comparation_product.xlsx
+++ b/tests/fixtures/comparation_product.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carlosherrero/projects/connect-cli/tests/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EC4C238-7306-0641-9EFA-135853587078}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE978CB5-A50F-044B-A2D0-C7A0893BB90E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" firstSheet="3" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3413,7 +3413,7 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
LITE-24215: Support templates of type 'pending'
</commit_message>
<xml_diff>
--- a/tests/fixtures/comparation_product.xlsx
+++ b/tests/fixtures/comparation_product.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carlosherrero/projects/connect-cli/tests/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC5B6949-5716-BC42-8A16-2284514DADF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B2D6FD4-8C0D-844E-84F0-148BD0D26A34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General Information" sheetId="1" r:id="rId1"/>
@@ -2145,7 +2145,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB98"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -3420,7 +3420,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62DD5574-F1F3-8943-BAA8-7E6A93E385BA}">
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
@@ -4989,7 +4989,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5175,7 +5175,7 @@
   </sheetData>
   <dataValidations count="3">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E2:E7" xr:uid="{00000000-0002-0000-0400-000002000000}">
-      <formula1>"fulfillment,inquire"</formula1>
+      <formula1>"pending,fulfillment,inquire"</formula1>
     </dataValidation>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D2:D7" xr:uid="{00000000-0002-0000-0400-000001000000}">
       <formula1>"asset,tier1,tier2"</formula1>

</xml_diff>

<commit_message>
LITE-29353: Added ProductMessage compatability on product export, sync and clone cmds
</commit_message>
<xml_diff>
--- a/tests/fixtures/comparation_product.xlsx
+++ b/tests/fixtures/comparation_product.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rselekh00/Development/connect-cli/tests/fixtures/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/esalog00/Work/github/connect-cli/tests/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DB5E821-FEA5-9F46-9019-2D96FAD4B772}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E6B23FA-DC46-D24F-A3E3-B5F29E22DE1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17180" firstSheet="5" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General Information" sheetId="1" r:id="rId1"/>
@@ -27,13 +27,14 @@
     <sheet name="Translations" sheetId="17" r:id="rId12"/>
     <sheet name="FA (TRN-1079-0833-9890)" sheetId="19" r:id="rId13"/>
     <sheet name="ES-AR (TRN-1079-0833-9891)" sheetId="20" r:id="rId14"/>
+    <sheet name="Messages" sheetId="21" r:id="rId15"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1250" uniqueCount="510">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1263" uniqueCount="518">
   <si>
     <t>Product information</t>
   </si>
@@ -1723,6 +1724,30 @@
   </si>
   <si>
     <t>Pay-as-you-go late charges support</t>
+  </si>
+  <si>
+    <t>External ID</t>
+  </si>
+  <si>
+    <t>Auto</t>
+  </si>
+  <si>
+    <t>error1</t>
+  </si>
+  <si>
+    <t>The value does not exists</t>
+  </si>
+  <si>
+    <t>error2</t>
+  </si>
+  <si>
+    <t>The operation is not possible</t>
+  </si>
+  <si>
+    <t>PRDMSG-276-377-545-0001</t>
+  </si>
+  <si>
+    <t>PRDMSG-276-377-545-0002</t>
   </si>
 </sst>
 </file>
@@ -4613,11 +4638,77 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80CABDDE-EF7F-F44E-96A2-BE56A6F537A3}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>510</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>516</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
+        <v>512</v>
+      </c>
+      <c r="D2" t="s">
+        <v>513</v>
+      </c>
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>517</v>
+      </c>
+      <c r="B3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" t="s">
+        <v>514</v>
+      </c>
+      <c r="D3" t="s">
+        <v>515</v>
+      </c>
+      <c r="E3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>

</xml_diff>